<commit_message>
Changed the authoritative, single source of truth to change a "Triangle" from "Move 100" to "Move 275".
35 files were modified.  These are - documentation, the 13 F# and 15 C# files.  The changes are pretty easily identifiable in the code.
</commit_message>
<xml_diff>
--- a/SSoT/twolaat.xlsx
+++ b/SSoT/twolaat.xlsx
@@ -22,19 +22,13 @@
     <t>Name</t>
   </si>
   <si>
-    <t>HexValue</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>WayNumber</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
     <t>InitialValue</t>
+  </si>
+  <si>
+    <t>WayNumber</t>
   </si>
   <si>
     <t>DisplayWayNumber</t>
@@ -46,7 +40,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Black</t>
+    <t>HexValue</t>
   </si>
   <si>
     <t>Notes</t>
@@ -55,10 +49,22 @@
     <t>Advantages</t>
   </si>
   <si>
+    <t>Version</t>
+  </si>
+  <si>
     <t>Disadvantages</t>
   </si>
   <si>
+    <t>Position</t>
+  </si>
+  <si>
     <t>W01</t>
+  </si>
+  <si>
+    <t>0x0</t>
+  </si>
+  <si>
+    <t>Black</t>
   </si>
   <si>
     <t>#000000</t>
@@ -91,17 +97,26 @@
     <t>Green</t>
   </si>
   <si>
-    <t>In this design, a simple OO class represents the turtle,
-and the client talks to the turtle directly.</t>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>Degrees</t>
   </si>
   <si>
     <t>#00FF00</t>
   </si>
   <si>
-    <t>Position</t>
+    <t>Color</t>
   </si>
   <si>
-    <t>0x0</t>
+    <t>PenState</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>In this design, a simple OO class represents the turtle,
+and the client talks to the turtle directly.</t>
   </si>
   <si>
     <t>W02</t>
@@ -167,21 +182,6 @@
   </si>
   <si>
     <t>W05</t>
-  </si>
-  <si>
-    <t>Angle</t>
-  </si>
-  <si>
-    <t>Degrees</t>
-  </si>
-  <si>
-    <t>Color</t>
-  </si>
-  <si>
-    <t>PenState</t>
-  </si>
-  <si>
-    <t>Down</t>
   </si>
   <si>
     <t>05-TurtleAgent.fsx</t>
@@ -256,12 +256,6 @@
     <t>W08</t>
   </si>
   <si>
-    <t>Up</t>
-  </si>
-  <si>
-    <t>The pen is up (not drawing)</t>
-  </si>
-  <si>
     <t>08-StateMonad.fsx</t>
   </si>
   <si>
@@ -269,15 +263,6 @@
   </si>
   <si>
     <t>Batch oriented -- Using a state monad (computation expression)</t>
-  </si>
-  <si>
-    <t>The pne is down (drawing)</t>
-  </si>
-  <si>
-    <t>Moving</t>
-  </si>
-  <si>
-    <t>The pen is in motion</t>
   </si>
   <si>
     <t>In this design, the client uses the FP Turtle functions directly.
@@ -306,13 +291,28 @@
     <t>W10</t>
   </si>
   <si>
+    <t>Up</t>
+  </si>
+  <si>
     <t>10-EventSourcing.fsx</t>
+  </si>
+  <si>
+    <t>The pen is up (not drawing)</t>
   </si>
   <si>
     <t>EventSourcing</t>
   </si>
   <si>
     <t>Event sourcing -- Building state from a list of past events</t>
+  </si>
+  <si>
+    <t>The pne is down (drawing)</t>
+  </si>
+  <si>
+    <t>Moving</t>
+  </si>
+  <si>
+    <t>The pen is in motion</t>
   </si>
   <si>
     <t>In this design, the client sends a `Command` to a `CommandHandler`.
@@ -382,6 +382,38 @@
     <t>W14</t>
   </si>
   <si>
+    <t>14-AdtTurtle.fsx</t>
+  </si>
+  <si>
+    <t>AdtTurtle</t>
+  </si>
+  <si>
+    <t>Abstract Data Turtle - a private type with an associated module of functions</t>
+  </si>
+  <si>
+    <t>In this design, the details of the turtle structure is hidden from the client,
+so the it could be changed without breaking any code.
+See https://www.reddit.com/r/fsharp/comments/36s0zr/structuring_f_programs_with_abstract_data_types/?
+for more on ADTs in F#.</t>
+  </si>
+  <si>
+    <t>W15</t>
+  </si>
+  <si>
+    <t>15-CapabilityBasedTurtle.fsx</t>
+  </si>
+  <si>
+    <t>CapabilityBasedTurtle</t>
+  </si>
+  <si>
+    <t>API with capabilities</t>
+  </si>
+  <si>
+    <t>In this design, the turtle exposes a list of functions (capabilities) after each action.
+These are the ONLY actions available to the client
+More on capability-based security at http://fsharpforfunandprofit.com/posts/capability-based-security/</t>
+  </si>
+  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -394,9 +426,6 @@
     <t>Parameter2Type</t>
   </si>
   <si>
-    <t>14-AdtTurtle.fsx</t>
-  </si>
-  <si>
     <t>Min</t>
   </si>
   <si>
@@ -406,28 +435,13 @@
     <t>APIName</t>
   </si>
   <si>
-    <t>AdtTurtle</t>
-  </si>
-  <si>
     <t>APIArgument</t>
-  </si>
-  <si>
-    <t>Abstract Data Turtle - a private type with an associated module of functions</t>
-  </si>
-  <si>
-    <t>In this design, the details of the turtle structure is hidden from the client,
-so the it could be changed without breaking any code.
-See https://www.reddit.com/r/fsharp/comments/36s0zr/structuring_f_programs_with_abstract_data_types/?
-for more on ADTs in F#.</t>
   </si>
   <si>
     <t>Move</t>
   </si>
   <si>
     <t>Moves the specified distance in whatever direction 'the turtle' is currently pointing.</t>
-  </si>
-  <si>
-    <t>W15</t>
   </si>
   <si>
     <t>Distance</t>
@@ -439,21 +453,7 @@
     <t>Turn</t>
   </si>
   <si>
-    <t>15-CapabilityBasedTurtle.fsx</t>
-  </si>
-  <si>
     <t>Turn the specified degrees from the current position</t>
-  </si>
-  <si>
-    <t>CapabilityBasedTurtle</t>
-  </si>
-  <si>
-    <t>API with capabilities</t>
-  </si>
-  <si>
-    <t>In this design, the turtle exposes a list of functions (capabilities) after each action.
-These are the ONLY actions available to the client
-More on capability-based security at http://fsharpforfunandprofit.com/posts/capability-based-security/</t>
   </si>
   <si>
     <t>PenUp</t>
@@ -618,14 +618,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
     <fill>
@@ -654,10 +654,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -667,20 +667,20 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -699,27 +699,27 @@
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="7" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -727,7 +727,7 @@
     <xf borderId="0" fillId="5" fontId="6" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -783,143 +783,143 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
     </row>
     <row r="3">
       <c r="A3" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
     </row>
     <row r="5">
       <c r="A5" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5" t="str">
         <f t="shared" ref="B6:B19" si="1">CONCATENATE("Way ",right(A6,2))</f>
@@ -931,10 +931,10 @@
       <c r="D6" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="12" t="s">
         <v>55</v>
       </c>
       <c r="G6" s="9"/>
@@ -954,10 +954,10 @@
       <c r="D7" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="12" t="s">
         <v>60</v>
       </c>
       <c r="G7" s="9"/>
@@ -977,10 +977,10 @@
       <c r="D8" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="12" t="s">
         <v>60</v>
       </c>
       <c r="G8" s="9"/>
@@ -1000,10 +1000,10 @@
       <c r="D9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="12" t="s">
         <v>68</v>
       </c>
       <c r="G9" s="9"/>
@@ -1023,10 +1023,10 @@
       <c r="D10" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="12" t="s">
         <v>68</v>
       </c>
       <c r="G10" s="9"/>
@@ -1041,61 +1041,61 @@
         <v>Way 08</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="F11" s="12" t="s">
         <v>76</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>81</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="13"/>
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B12" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 09</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B13" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 10</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F13" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>91</v>
       </c>
       <c r="G13" s="13"/>
@@ -1115,10 +1115,10 @@
       <c r="D14" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="12" t="s">
         <v>96</v>
       </c>
       <c r="G14" s="13"/>
@@ -1138,10 +1138,10 @@
       <c r="D15" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="12" t="s">
         <v>101</v>
       </c>
       <c r="G15" s="13"/>
@@ -1161,10 +1161,10 @@
       <c r="D16" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="12" t="s">
         <v>106</v>
       </c>
       <c r="G16" s="13"/>
@@ -1184,10 +1184,10 @@
       <c r="D17" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="12" t="s">
         <v>106</v>
       </c>
       <c r="G17" s="13"/>
@@ -1202,74 +1202,74 @@
         <v>Way 14</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>121</v>
+        <v>111</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
     </row>
     <row r="19">
       <c r="A19" s="6" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B19" s="5" t="str">
         <f t="shared" si="1"/>
         <v>Way 15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>132</v>
+        <v>116</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
     </row>
     <row r="20">
       <c r="A20" s="13"/>
-      <c r="E20" s="7"/>
+      <c r="E20" s="12"/>
       <c r="F20" s="16"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
     <row r="21">
       <c r="A21" s="13"/>
-      <c r="E21" s="7"/>
+      <c r="E21" s="12"/>
       <c r="F21" s="16"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
     </row>
     <row r="22">
       <c r="A22" s="13"/>
-      <c r="E22" s="7"/>
+      <c r="E22" s="12"/>
       <c r="F22" s="16"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
     </row>
     <row r="23">
       <c r="A23" s="13"/>
-      <c r="E23" s="7"/>
+      <c r="E23" s="12"/>
       <c r="F23" s="16"/>
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
     <row r="24">
       <c r="A24" s="13"/>
-      <c r="E24" s="7"/>
+      <c r="E24" s="12"/>
       <c r="F24" s="16"/>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
@@ -8123,52 +8123,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>27</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="C3" s="9">
         <v>0.0</v>
@@ -8176,24 +8176,24 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>9</v>
+        <v>29</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>51</v>
+        <v>30</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6">
@@ -11201,40 +11201,40 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="5">
         <v>1.0</v>
@@ -11242,10 +11242,10 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" s="5">
         <v>1.0</v>
@@ -11253,10 +11253,10 @@
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5">
         <v>1.0</v>
@@ -11264,10 +11264,10 @@
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C5" s="8">
         <v>2.0</v>
@@ -11318,10 +11318,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -11349,10 +11349,10 @@
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C2" s="5">
         <v>1.0</v>
@@ -11360,10 +11360,10 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="C3" s="5">
         <v>1.0</v>
@@ -11371,10 +11371,10 @@
     </row>
     <row r="4">
       <c r="A4" s="8" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C4" s="8">
         <v>2.0</v>
@@ -11428,67 +11428,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
+        <v>126</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -11502,21 +11502,21 @@
         <v>1000.0</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -11530,7 +11530,7 @@
         <v>360.0</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4">
@@ -11549,7 +11549,7 @@
         <v>135</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5">
@@ -11568,7 +11568,7 @@
         <v>135</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
@@ -11579,7 +11579,7 @@
         <v>139</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>140</v>
@@ -11653,10 +11653,10 @@
         <v>146</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -12294,13 +12294,13 @@
         <v>156</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>157</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
@@ -12430,7 +12430,7 @@
         <v>166</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>167</v>
@@ -12464,10 +12464,10 @@
         <v>Triangle</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C2" s="21">
-        <v>100.0</v>
+        <v>275.0</v>
       </c>
       <c r="E2" s="22" t="str">
         <f>vlookup(B2,TurtleCommands!A$2:C7,3,false)</f>
@@ -12502,7 +12502,7 @@
         <v>Triangle</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C3" s="21">
         <v>120.0</v>
@@ -12540,10 +12540,10 @@
         <v>Triangle</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C4" s="21">
-        <v>100.0</v>
+        <v>275.0</v>
       </c>
       <c r="E4" s="22" t="str">
         <f>vlookup(B4,TurtleCommands!A$2:C9,3,false)</f>
@@ -12578,7 +12578,7 @@
         <v>Triangle</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C5" s="21">
         <v>120.0</v>
@@ -12616,10 +12616,10 @@
         <v>Triangle</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C6" s="21">
-        <v>100.0</v>
+        <v>275.0</v>
       </c>
       <c r="E6" s="22" t="str">
         <f>vlookup(B6,TurtleCommands!A$2:C11,3,false)</f>
@@ -12654,7 +12654,7 @@
         <v>Triangle</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C7" s="21">
         <v>120.0</v>
@@ -12736,7 +12736,7 @@
         <v>138</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="22" t="str">
@@ -12772,7 +12772,7 @@
         <v>ThreeLines</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C10" s="25">
         <v>100.0</v>
@@ -12850,7 +12850,7 @@
         <v>ThreeLines</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C12" s="25">
         <v>90.0</v>
@@ -12889,7 +12889,7 @@
         <v>ThreeLines</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C13" s="25">
         <v>100.0</v>
@@ -12928,7 +12928,7 @@
         <v>ThreeLines</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C14" s="25">
         <v>90.0</v>
@@ -13009,7 +13009,7 @@
         <v>138</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="22" t="str">
@@ -13045,7 +13045,7 @@
         <v>ThreeLines</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C17" s="25">
         <v>100.0</v>
@@ -13123,7 +13123,7 @@
         <v>ThreeLines</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C19" s="25">
         <v>90.0</v>
@@ -13162,7 +13162,7 @@
         <v>ThreeLines</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C20" s="25">
         <v>100.0</v>
@@ -13201,7 +13201,7 @@
         <v>ThreeLines</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C21" s="25">
         <v>90.0</v>
@@ -13282,7 +13282,7 @@
         <v>138</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D23" s="24"/>
       <c r="E23" s="22" t="str">
@@ -13318,7 +13318,7 @@
         <v>ThreeLines</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C24" s="25">
         <v>45.0</v>
@@ -13357,7 +13357,7 @@
         <v>ThreeLines</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C25" s="25">
         <v>100.0</v>
@@ -13396,7 +13396,7 @@
         <v>Box</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C26" s="31">
         <v>100.0</v>
@@ -13435,7 +13435,7 @@
         <v>Box</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C27" s="31">
         <v>90.0</v>
@@ -13474,7 +13474,7 @@
         <v>Box</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C28" s="31">
         <v>100.0</v>
@@ -13513,7 +13513,7 @@
         <v>Box</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C29" s="31">
         <v>90.0</v>
@@ -13552,7 +13552,7 @@
         <v>Box</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C30" s="31">
         <v>100.0</v>
@@ -13591,7 +13591,7 @@
         <v>Box</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C31" s="31">
         <v>90.0</v>
@@ -13630,7 +13630,7 @@
         <v>Box</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C32" s="31">
         <v>100.0</v>
@@ -13669,7 +13669,7 @@
         <v>Box</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C33" s="31">
         <v>90.0</v>

</xml_diff>